<commit_message>
Minimum Nr 3005 eingeführt, damit Sortierung etwas anzeigt
</commit_message>
<xml_diff>
--- a/Preise.xlsx
+++ b/Preise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\VBA Tage\VBA Tage 2019\VBA-Tanker\VBATanker\Downloads\Beispiel 10722\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F548A3-4C89-4E7C-BAE2-6101907E738A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2E1C41-FD4A-4787-B5FA-EB31F4249F87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9293138A-368B-43BB-93D9-9979760E3176}"/>
+    <workbookView xWindow="-28500" yWindow="2580" windowWidth="7950" windowHeight="11385" xr2:uid="{9293138A-368B-43BB-93D9-9979760E3176}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -393,7 +393,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +480,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>5005</v>
+        <v>3005</v>
       </c>
       <c r="B11">
         <v>3</v>

</xml_diff>